<commit_message>
DRAFT4 - version sent to Terry Stouch. Edits and extra SI figures from IEN.
</commit_message>
<xml_diff>
--- a/figures/NMR_microstates/SM07_SM14_protonation_sites_edited.xlsx
+++ b/figures/NMR_microstates/SM07_SM14_protonation_sites_edited.xlsx
@@ -250,11 +250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2119719320"/>
-        <c:axId val="-2119712168"/>
+        <c:axId val="-2135777848"/>
+        <c:axId val="-2126044248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2119719320"/>
+        <c:axId val="-2135777848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -293,12 +293,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119712168"/>
+        <c:crossAx val="-2126044248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2119712168"/>
+        <c:axId val="-2126044248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="145.0"/>
@@ -343,7 +343,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119719320"/>
+        <c:crossAx val="-2135777848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -475,11 +475,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2140207144"/>
-        <c:axId val="2141133560"/>
+        <c:axId val="-2129724856"/>
+        <c:axId val="-2124126360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140207144"/>
+        <c:axId val="-2129724856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,12 +518,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141133560"/>
+        <c:crossAx val="-2124126360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141133560"/>
+        <c:axId val="-2124126360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="220.0"/>
@@ -595,7 +595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140207144"/>
+        <c:crossAx val="-2129724856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -727,11 +727,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142440392"/>
-        <c:axId val="2141026248"/>
+        <c:axId val="-2124081080"/>
+        <c:axId val="-2130095752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142440392"/>
+        <c:axId val="-2124081080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,12 +775,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141026248"/>
+        <c:crossAx val="-2130095752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141026248"/>
+        <c:axId val="-2130095752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130.0"/>
@@ -853,7 +853,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142440392"/>
+        <c:crossAx val="-2124081080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -915,8 +915,26 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>SM07_fitting!$E$6:$E$10</c:f>
@@ -965,7 +983,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -982,11 +1000,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1036,7 +1068,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1053,8 +1085,24 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="008000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>SM07_fitting!$E$6:$E$10</c:f>
@@ -1103,7 +1151,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1113,11 +1161,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2114030824"/>
-        <c:axId val="-2053977576"/>
+        <c:axId val="-2124128184"/>
+        <c:axId val="-2125898264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2114030824"/>
+        <c:axId val="-2124128184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,13 +1197,13 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="-2053977576"/>
+        <c:crossAx val="-2125898264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2053977576"/>
+        <c:axId val="-2125898264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="240.0"/>
@@ -1193,7 +1241,7 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="-2114030824"/>
+        <c:crossAx val="-2124128184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1425,11 +1473,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2120734488"/>
-        <c:axId val="-2120809384"/>
+        <c:axId val="-2131583800"/>
+        <c:axId val="-2131576248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2120734488"/>
+        <c:axId val="-2131583800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,12 +1521,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120809384"/>
+        <c:crossAx val="-2131576248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2120809384"/>
+        <c:axId val="-2131576248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250.0"/>
@@ -1530,7 +1578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120734488"/>
+        <c:crossAx val="-2131583800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1711,11 +1759,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2115617656"/>
-        <c:axId val="-2120557512"/>
+        <c:axId val="-2127047128"/>
+        <c:axId val="-2127041672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2115617656"/>
+        <c:axId val="-2127047128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12.0"/>
@@ -1761,12 +1809,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120557512"/>
+        <c:crossAx val="-2127041672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2120557512"/>
+        <c:axId val="-2127041672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="176.0"/>
@@ -1818,7 +1866,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115617656"/>
+        <c:crossAx val="-2127047128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2005,11 +2053,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2120959448"/>
-        <c:axId val="2142337688"/>
+        <c:axId val="-2127013416"/>
+        <c:axId val="-2127005608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2120959448"/>
+        <c:axId val="-2127013416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12.0"/>
@@ -2055,12 +2103,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142337688"/>
+        <c:crossAx val="-2127005608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142337688"/>
+        <c:axId val="-2127005608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2110,7 +2158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120959448"/>
+        <c:crossAx val="-2127013416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2179,8 +2227,24 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>SM14_Acetonitrile_fitting_2!$C$8:$C$20</c:f>
@@ -2277,7 +2341,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2294,11 +2358,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2396,7 +2474,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2413,8 +2491,24 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400"/>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:ln>
           </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="008000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>SM14_Acetonitrile_fitting_2!$C$8:$C$20</c:f>
@@ -2511,7 +2605,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2521,11 +2615,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2039406040"/>
-        <c:axId val="-2019637288"/>
+        <c:axId val="-2124087960"/>
+        <c:axId val="-2135792776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2039406040"/>
+        <c:axId val="-2124087960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2557,13 +2651,13 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="-2019637288"/>
+        <c:crossAx val="-2135792776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2019637288"/>
+        <c:axId val="-2135792776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250.0"/>
@@ -2601,7 +2695,7 @@
         <c:spPr>
           <a:ln w="19050"/>
         </c:spPr>
-        <c:crossAx val="-2039406040"/>
+        <c:crossAx val="-2124087960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3272,7 +3366,7 @@
   <dimension ref="E5:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3378,7 +3472,7 @@
   <dimension ref="C7:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>